<commit_message>
Refactor quick resolver value
</commit_message>
<xml_diff>
--- a/tests/data/test_data_04.xlsx
+++ b/tests/data/test_data_04.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wizz/Documents/Projects/excelcy/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBBE37E-88E1-5741-9CC8-7B8341D54600}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743DBD1B-710D-FD4C-8D6B-D3459EC36031}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>text</t>
   </si>
@@ -176,16 +176,10 @@
     <t>save_nlp</t>
   </si>
   <si>
-    <t>save_storage</t>
-  </si>
-  <si>
     <t>args</t>
   </si>
   <si>
     <t>file_path=person.xlsx, label=PERSON</t>
-  </si>
-  <si>
-    <t>file_path=[storage_name].xlsx</t>
   </si>
   <si>
     <t>file_path=[tmp]/nlp/data-[date][time]</t>
@@ -531,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92BBB3E5-6C1D-7646-B12D-3BE01DC03441}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -556,7 +550,7 @@
         <v>47</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>46</v>
@@ -573,7 +567,7 @@
         <v>49</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -606,10 +600,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -620,21 +611,10 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>